<commit_message>
Now keeping one run and results overview, not per folder
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C47CA6-CE53-45D0-9917-D60777298CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F96B0-6861-4488-B01E-C9C024A47952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +112,69 @@
   </si>
   <si>
     <t>failed?</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Renewed version</t>
+  </si>
+  <si>
+    <t>TODO after</t>
+  </si>
+  <si>
+    <t>annotation, DEG, pseudotime</t>
+  </si>
+  <si>
+    <t>2022-06-10 16-29-41</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_N</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_A</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_C</t>
+  </si>
+  <si>
+    <t>integration (old/new selection), annotation, DEG, pseudotime</t>
+  </si>
+  <si>
+    <t>rerun SCTv2 corrected pipeline</t>
+  </si>
+  <si>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>Pipe_SCTv2_corrected_13-06</t>
+  </si>
+  <si>
+    <t>2022-06-13 13-32-07</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_A + BL_C new selection</t>
+  </si>
+  <si>
+    <t>2022-06-13 13-33-22</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_A + BL_C old selection</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_N + BL_C new selection</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_N + BL_C old selection</t>
+  </si>
+  <si>
+    <t>2022-06-13 13-34-02</t>
+  </si>
+  <si>
+    <t>2022-06-13 13-35-10</t>
   </si>
 </sst>
 </file>
@@ -429,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,9 +504,11 @@
     <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -459,8 +524,14 @@
       <c r="E1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -473,8 +544,11 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -487,8 +561,11 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -501,8 +578,11 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -515,8 +595,11 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -529,8 +612,11 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -543,8 +629,11 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -557,8 +646,17 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -571,16 +669,171 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to run SCTv2 correctd BL_A for DEG, got error, look into DEG errors for individual DEG runs? does this also happen for integrated data?
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F96B0-6861-4488-B01E-C9C024A47952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -111,9 +105,6 @@
     <t>SCTv2 BL_A + BL_C with new visualizations/selection</t>
   </si>
   <si>
-    <t>failed?</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -175,12 +166,33 @@
   </si>
   <si>
     <t>2022-06-13 13-35-10</t>
+  </si>
+  <si>
+    <t>Neurolucida results</t>
+  </si>
+  <si>
+    <t>2022-06-13 14-02-37</t>
+  </si>
+  <si>
+    <t>annotation, pseudotime</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Error in ValidateCellGroups(object = object, cells.1 = cells.1, cells.2 = cells.2,  : Cell group 2 is empty - no cells with identity class  Calls: sourceWithProgress ... FindMarkers -&gt; FindMarkers.default -&gt; ValidateCellGroups3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -307,7 +319,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -484,18 +496,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +520,7 @@
     <col min="7" max="7" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -522,16 +534,19 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -545,10 +560,10 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -562,10 +577,10 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -579,10 +594,10 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -596,10 +611,10 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -613,10 +628,10 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -630,10 +645,10 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -647,16 +662,16 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -670,21 +685,21 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -693,147 +708,178 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
-      </c>
-      <c r="F14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest log on laptop
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F96B0-6861-4488-B01E-C9C024A47952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A4D2C0-FC1B-41EB-86CB-788388A458A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Running SCTv2 corrected data for annotation, Kriegstein to Rdata
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2005A9C-5533-4F2B-A5C0-5ADA6CE4C0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +57,6 @@
     <t xml:space="preserve">SCTv2 old selection </t>
   </si>
   <si>
-    <t>RData</t>
-  </si>
-  <si>
     <t>2022-06-09 17-36-28</t>
   </si>
   <si>
@@ -144,15 +147,9 @@
     <t>Pipe_SCTv2_corrected_13-06</t>
   </si>
   <si>
-    <t>2022-06-13 13-32-07</t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_A + BL_C new selection</t>
   </si>
   <si>
-    <t>2022-06-13 13-33-22</t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_A + BL_C old selection</t>
   </si>
   <si>
@@ -162,12 +159,6 @@
     <t>SCTv2 corrected BL_N + BL_C old selection</t>
   </si>
   <si>
-    <t>2022-06-13 13-34-02</t>
-  </si>
-  <si>
-    <t>2022-06-13 13-35-10</t>
-  </si>
-  <si>
     <t>Neurolucida results</t>
   </si>
   <si>
@@ -183,16 +174,46 @@
     <t>error</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Error in ValidateCellGroups(object = object, cells.1 = cells.1, cells.2 = cells.2,  : Cell group 2 is empty - no cells with identity class  Calls: sourceWithProgress ... FindMarkers -&gt; FindMarkers.default -&gt; ValidateCellGroups3</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-13 14-46-51</t>
+  </si>
+  <si>
+    <t>DEG, pseudotime</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected new selection</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected new post selection</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected old post selection</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected old selection</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-13 14-50-40</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-13 14-55-08</t>
+  </si>
+  <si>
+    <t>rerun SCTv2 corrected pipeline (integrated)</t>
+  </si>
+  <si>
+    <t>rerun SCTv2 corrected pipeline (individual + integrated)</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-13 14-56-28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,18 +517,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,16 +555,16 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -557,15 +578,15 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -577,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -585,67 +606,67 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,22 +674,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,22 +697,22 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -699,16 +720,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -716,19 +737,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
         <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -736,19 +757,19 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,19 +777,19 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -776,19 +797,19 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -796,19 +817,19 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -816,19 +837,19 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -836,50 +857,125 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
         <v>53</v>
       </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
         <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed script and reran, added run to log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2005A9C-5533-4F2B-A5C0-5ADA6CE4C0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD44D32-8908-4778-8F51-C2AF563907DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,7 +207,7 @@
     <t>rerun SCTv2 corrected pipeline (individual + integrated)</t>
   </si>
   <si>
-    <t>SingleR_RData_2022-06-13 14-56-28</t>
+    <t>SingleR_RData_2022-06-13 15-00-51</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Run and log of SCTv2 corrected BL_A + BL_C new post selection
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD44D32-8908-4778-8F51-C2AF563907DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -208,12 +202,21 @@
   </si>
   <si>
     <t>SingleR_RData_2022-06-13 15-00-51</t>
+  </si>
+  <si>
+    <t>2022-06-13 15-18-49</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_A + BL_C new post selection</t>
+  </si>
+  <si>
+    <t>pseudotime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,18 +520,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,6 +981,26 @@
         <v>51</v>
       </c>
     </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Running DEG and added runs to log, also added total SCTv2 pipetimeline to log file
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851B3979-24B3-4C2F-8BB7-B6BBD797D2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="logs" sheetId="1" r:id="rId1"/>
+    <sheet name="SCTv2 pipeline runtime" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -211,12 +218,78 @@
   </si>
   <si>
     <t>pseudotime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">did I put new selection on too? </t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_A + BL_C old post selection</t>
+  </si>
+  <si>
+    <t>2022-06-14 07-42-05</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>BL_N</t>
+  </si>
+  <si>
+    <t>BL_A</t>
+  </si>
+  <si>
+    <t>BL_C</t>
+  </si>
+  <si>
+    <t>in parallel</t>
+  </si>
+  <si>
+    <t>integration old selection</t>
+  </si>
+  <si>
+    <t>integration new selection</t>
+  </si>
+  <si>
+    <t>BL_N + BL_C</t>
+  </si>
+  <si>
+    <t>BL_A + BL_C</t>
+  </si>
+  <si>
+    <t>time (min)</t>
+  </si>
+  <si>
+    <t>annotation old selection</t>
+  </si>
+  <si>
+    <t>annotation old post selection</t>
+  </si>
+  <si>
+    <t>annotation new post selection</t>
+  </si>
+  <si>
+    <t>annotation new selection</t>
+  </si>
+  <si>
+    <t>individual + integration</t>
+  </si>
+  <si>
+    <t>sample(s)</t>
+  </si>
+  <si>
+    <t>278/515</t>
+  </si>
+  <si>
+    <t>DEGs</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,8 +319,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,18 +594,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,6 +1075,230 @@
         <v>63</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F9FEED-2ED0-4252-8854-390CEAC37BF3}">
+  <dimension ref="B1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="1">
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="1">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1">
+        <v>278</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Running SCTv2 corrected BL_N + BL_C old (post) selection DEG
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18827CE5-5C72-4A2E-B77E-1CBD389B2DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -220,9 +214,6 @@
     <t>pseudotime</t>
   </si>
   <si>
-    <t xml:space="preserve">did I put new selection on too? </t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_A + BL_C old post selection</t>
   </si>
   <si>
@@ -284,12 +275,24 @@
   </si>
   <si>
     <t>2022-06-14 07-47-37</t>
+  </si>
+  <si>
+    <t>2022-06-13 16-27-52</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_N + BL_C old post selection</t>
+  </si>
+  <si>
+    <t>2022-06-14 14-45-40</t>
+  </si>
+  <si>
+    <t>2022-06-14 14-46-19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,18 +597,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,8 +1079,17 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
         <v>37</v>
@@ -1097,7 +1109,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
         <v>37</v>
@@ -1111,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -1123,6 +1135,46 @@
         <v>37</v>
       </c>
       <c r="G26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1132,7 +1184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F9FEED-2ED0-4252-8854-390CEAC37BF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1150,21 +1202,21 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
@@ -1175,7 +1227,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -1186,7 +1238,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1200,10 +1252,10 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
@@ -1211,10 +1263,10 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1">
         <v>32</v>
@@ -1222,10 +1274,10 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1">
         <v>37</v>
@@ -1233,10 +1285,10 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1">
         <v>37</v>
@@ -1247,10 +1299,10 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1">
         <v>515</v>
@@ -1261,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1">
         <v>277</v>
@@ -1272,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1">
         <v>275</v>
@@ -1283,23 +1335,23 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1">
         <v>278</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run and log update
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B683F1FA-C487-4DC7-A3F8-747B712478F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -205,9 +211,6 @@
     <t>SingleR_RData_2022-06-13 15-00-51</t>
   </si>
   <si>
-    <t>2022-06-13 15-18-49</t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_A + BL_C new post selection</t>
   </si>
   <si>
@@ -277,9 +280,6 @@
     <t>2022-06-14 07-47-37</t>
   </si>
   <si>
-    <t>2022-06-13 16-27-52</t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_N + BL_C old post selection</t>
   </si>
   <si>
@@ -287,12 +287,18 @@
   </si>
   <si>
     <t>2022-06-14 14-46-19</t>
+  </si>
+  <si>
+    <t>SCTv2 corrected BL_N + BL_C new post selection</t>
+  </si>
+  <si>
+    <t>2022-06-14 15-03-49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,18 +603,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,19 +1069,19 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
         <v>62</v>
-      </c>
-      <c r="F23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1083,7 +1089,7 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1095,7 +1101,7 @@
         <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,13 +1115,13 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
         <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1123,7 +1129,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -1135,7 +1141,7 @@
         <v>37</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1143,19 +1149,19 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F27" t="s">
         <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1163,7 +1169,7 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1175,7 +1181,24 @@
         <v>37</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1202,21 +1225,21 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
@@ -1227,7 +1250,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -1238,7 +1261,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1252,10 +1275,10 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
@@ -1263,10 +1286,10 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1">
         <v>32</v>
@@ -1274,10 +1297,10 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1">
         <v>37</v>
@@ -1285,10 +1308,10 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1">
         <v>37</v>
@@ -1299,10 +1322,10 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1">
         <v>515</v>
@@ -1313,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1">
         <v>277</v>
@@ -1324,7 +1347,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1">
         <v>275</v>
@@ -1335,23 +1358,23 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="1">
         <v>278</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed files and canceled run to prioritize rechunking for SingleR annotation of SCTv2 data
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75050EA6-C25F-48A4-9A2F-F2B954102211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553F5CAA-1FAC-4EED-960A-6F438891EFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -287,12 +287,6 @@
   </si>
   <si>
     <t>SCTv2 corrected BL_N + BL_C new post selection</t>
-  </si>
-  <si>
-    <t>2022-06-14 15-03-49</t>
-  </si>
-  <si>
-    <t>2022-06-14 15-16-04</t>
   </si>
 </sst>
 </file>
@@ -614,7 +608,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,9 +1182,6 @@
       <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B29" t="s">
-        <v>87</v>
-      </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
@@ -1207,9 +1198,6 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
-      </c>
-      <c r="B30" t="s">
-        <v>88</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Rerunning SCTv2 corrected annotation after rechunking Kriegstein ref data, both with corrected parameters
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA853C9-63D5-4B67-9D1C-112E256848F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0326F509-79C3-49BE-9840-256D72C2118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -289,9 +289,6 @@
     <t>SCTv2 corrected BL_N + BL_C new post selection</t>
   </si>
   <si>
-    <t>2022-06-14 16-10-45_chunks</t>
-  </si>
-  <si>
     <t>chunking Kriegstein</t>
   </si>
   <si>
@@ -302,6 +299,21 @@
   </si>
   <si>
     <t>2022-06-14 19-06-41</t>
+  </si>
+  <si>
+    <t>chunks_25</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-15 09-10-25</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-15 09-11-29</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-15 09-13-25</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-15 09-14-33</t>
   </si>
 </sst>
 </file>
@@ -620,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,6 +1018,9 @@
       <c r="D19" t="s">
         <v>52</v>
       </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
       <c r="F19" t="s">
         <v>58</v>
       </c>
@@ -1026,6 +1041,9 @@
       <c r="D20" t="s">
         <v>53</v>
       </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
       <c r="F20" t="s">
         <v>58</v>
       </c>
@@ -1046,6 +1064,9 @@
       <c r="D21" t="s">
         <v>55</v>
       </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
       <c r="F21" t="s">
         <v>59</v>
       </c>
@@ -1066,6 +1087,9 @@
       <c r="D22" t="s">
         <v>54</v>
       </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
       <c r="F22" t="s">
         <v>58</v>
       </c>
@@ -1198,7 +1222,7 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -1218,7 +1242,7 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1238,16 +1262,99 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
         <v>87</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="s">
-        <v>89</v>
-      </c>
       <c r="F31" t="s">
         <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerunning errored DEG and updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0326F509-79C3-49BE-9840-256D72C2118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -283,9 +277,6 @@
     <t>2022-06-14 14-45-40</t>
   </si>
   <si>
-    <t>2022-06-14 14-46-19</t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_N + BL_C new post selection</t>
   </si>
   <si>
@@ -295,9 +286,6 @@
     <t>SCTv2 corrected pipeline rechunking Kriegstein ref data</t>
   </si>
   <si>
-    <t>2022-06-14 17-10-47</t>
-  </si>
-  <si>
     <t>2022-06-14 19-06-41</t>
   </si>
   <si>
@@ -314,12 +302,18 @@
   </si>
   <si>
     <t>SingleR_RData_2022-06-15 09-14-33</t>
+  </si>
+  <si>
+    <t>2022-06-15 12-12-24</t>
+  </si>
+  <si>
+    <t>2022-06-15 12-12-56</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -624,18 +618,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,13 +1196,16 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" t="s">
         <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
       </c>
       <c r="F28" t="s">
         <v>37</v>
@@ -1222,13 +1219,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
         <v>37</v>
@@ -1242,13 +1239,16 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" t="s">
         <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
       </c>
       <c r="F30" t="s">
         <v>37</v>
@@ -1262,13 +1262,13 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
         <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>88</v>
       </c>
       <c r="F31" t="s">
         <v>37</v>
@@ -1282,7 +1282,7 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -1302,7 +1302,7 @@
         <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -1322,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1342,7 +1342,7 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -1363,7 +1363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update run and log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -304,10 +304,13 @@
     <t>SingleR_RData_2022-06-15 09-14-33</t>
   </si>
   <si>
-    <t>2022-06-15 12-12-24</t>
-  </si>
-  <si>
-    <t>2022-06-15 12-12-56</t>
+    <t>?</t>
+  </si>
+  <si>
+    <t>2022-06-15 16-04-57</t>
+  </si>
+  <si>
+    <t>2022-06-15 16-05-31</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -629,7 +632,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,6 +1187,9 @@
       <c r="D27" t="s">
         <v>83</v>
       </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
       <c r="F27" t="s">
         <v>37</v>
       </c>
@@ -1196,16 +1202,13 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" t="s">
         <v>43</v>
-      </c>
-      <c r="E28" t="s">
-        <v>48</v>
       </c>
       <c r="F28" t="s">
         <v>37</v>
@@ -1239,16 +1242,13 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" t="s">
         <v>42</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
       </c>
       <c r="F30" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated DE analysis condition markers with checking the original identities within subsets to have at least 3 cells such that FindMarkers can run successfully
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CC73F2-6724-490A-AE32-EC73D8BBCC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -304,16 +298,16 @@
     <t>SingleR_RData_2022-06-15 09-14-33</t>
   </si>
   <si>
-    <t>2022-06-15 16-04-57</t>
-  </si>
-  <si>
-    <t>2022-06-15 16-05-31</t>
+    <t>2022-06-20 11-38-02</t>
+  </si>
+  <si>
+    <t>2022-06-20 11-38-33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,18 +612,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1190,7 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1236,7 +1230,7 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1357,7 +1351,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
New temps for running and updated log with active runs
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE538A5-6650-455C-8806-146EA654993E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -298,16 +304,34 @@
     <t>SingleR_RData_2022-06-15 09-14-33</t>
   </si>
   <si>
-    <t>2022-06-20 11-38-33</t>
-  </si>
-  <si>
-    <t>2022-06-21 15-05-59</t>
+    <t>Kriegstein</t>
+  </si>
+  <si>
+    <t>SingleR visualization</t>
+  </si>
+  <si>
+    <t>SCTv2 preSelection aggrFalse labels score.max</t>
+  </si>
+  <si>
+    <t>SCTv2 preSelection aggrTrue labels score.max</t>
+  </si>
+  <si>
+    <t>SCTv2 postSelection aggrFalse labels score.max</t>
+  </si>
+  <si>
+    <t>SCTv2 postSelection aggrTrue labels score.max</t>
+  </si>
+  <si>
+    <t>2022-06-22 17-28-57</t>
+  </si>
+  <si>
+    <t>2022-06-22 17-29-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -612,18 +636,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1214,7 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1230,7 +1254,7 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1343,6 +1367,62 @@
       </c>
       <c r="G35" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1351,7 +1431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Renewed temps for rerun SCTv2 because of error in Kriegstein-SingleR heatmap visualizations, updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C40912-9632-4ADF-85D1-1226A47D3BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E1C2C-69FA-48EC-B37C-92218463ECAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -310,22 +310,58 @@
     <t>SingleR visualization</t>
   </si>
   <si>
-    <t>SCTv2 preSelection aggrFalse labels score.max</t>
-  </si>
-  <si>
-    <t>SCTv2 preSelection aggrTrue labels score.max</t>
-  </si>
-  <si>
-    <t>SCTv2 postSelection aggrFalse labels score.max</t>
-  </si>
-  <si>
-    <t>SCTv2 postSelection aggrTrue labels score.max</t>
-  </si>
-  <si>
-    <t>2022-06-22 17-33-35</t>
-  </si>
-  <si>
-    <t>2022-06-22 17-33-56</t>
+    <t>SCTv2 preselection aggrFalse meanLabelScore</t>
+  </si>
+  <si>
+    <t>SCTv2 preselection aggrTrue meanLabelScore</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>postselection data failing in visualization, probably wrong data in Kriegstein to SingleR so need to rerun (after organising parameters for visualization)</t>
+  </si>
+  <si>
+    <t>rerun</t>
+  </si>
+  <si>
+    <t>as desc</t>
+  </si>
+  <si>
+    <t>SCTv2 preselection aggrFalse maxLabelScore</t>
+  </si>
+  <si>
+    <t>SCTv2 preselection aggrTrue maxLabelScore</t>
+  </si>
+  <si>
+    <t>A + C</t>
+  </si>
+  <si>
+    <t>old selection</t>
+  </si>
+  <si>
+    <t>new selection</t>
+  </si>
+  <si>
+    <t>Pipe_SCTv2_23-06</t>
+  </si>
+  <si>
+    <t>N + C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>2022-06-23 16-03-44</t>
+  </si>
+  <si>
+    <t>2022-06-23 16-04-56</t>
   </si>
 </sst>
 </file>
@@ -644,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,12 +691,13 @@
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -671,22 +708,25 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -696,14 +736,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -713,14 +753,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -730,14 +770,14 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -747,14 +787,14 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -764,14 +804,14 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -781,14 +821,14 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -798,20 +838,20 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -821,20 +861,20 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -844,14 +884,14 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -861,17 +901,17 @@
       <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
       <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -881,17 +921,17 @@
       <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" t="s">
-        <v>37</v>
-      </c>
       <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -901,17 +941,17 @@
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
       <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -921,17 +961,17 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" t="s">
-        <v>37</v>
-      </c>
       <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -941,17 +981,17 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
       <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -961,17 +1001,17 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
       <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -981,17 +1021,17 @@
       <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>43</v>
       </c>
-      <c r="F17" t="s">
-        <v>37</v>
-      </c>
       <c r="G17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1001,23 +1041,23 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>48</v>
       </c>
-      <c r="F18" t="s">
-        <v>37</v>
-      </c>
       <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
         <v>46</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1027,20 +1067,20 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>38</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>58</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1050,20 +1090,20 @@
       <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>53</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>38</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>58</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1073,20 +1113,20 @@
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>55</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>38</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>59</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1096,20 +1136,20 @@
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>54</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>38</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>58</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1119,17 +1159,17 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="F23" t="s">
-        <v>37</v>
-      </c>
       <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1139,17 +1179,17 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>40</v>
       </c>
-      <c r="F24" t="s">
-        <v>37</v>
-      </c>
       <c r="G24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1159,17 +1199,17 @@
       <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>63</v>
       </c>
-      <c r="F25" t="s">
-        <v>37</v>
-      </c>
       <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1179,17 +1219,17 @@
       <c r="C26" t="s">
         <v>23</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>41</v>
       </c>
-      <c r="F26" t="s">
-        <v>37</v>
-      </c>
       <c r="G26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1199,17 +1239,17 @@
       <c r="C27" t="s">
         <v>23</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>83</v>
       </c>
-      <c r="F27" t="s">
-        <v>37</v>
-      </c>
       <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1219,17 +1259,17 @@
       <c r="C28" t="s">
         <v>23</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>43</v>
       </c>
-      <c r="F28" t="s">
-        <v>37</v>
-      </c>
       <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1239,17 +1279,17 @@
       <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>84</v>
       </c>
-      <c r="F29" t="s">
-        <v>37</v>
-      </c>
       <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1259,17 +1299,17 @@
       <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>42</v>
       </c>
-      <c r="F30" t="s">
-        <v>37</v>
-      </c>
       <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1279,17 +1319,17 @@
       <c r="C31" t="s">
         <v>85</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>86</v>
       </c>
-      <c r="F31" t="s">
-        <v>37</v>
-      </c>
       <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1299,17 +1339,17 @@
       <c r="C32" t="s">
         <v>8</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>53</v>
       </c>
-      <c r="F32" t="s">
-        <v>37</v>
-      </c>
       <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1319,17 +1359,17 @@
       <c r="C33" t="s">
         <v>8</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>54</v>
       </c>
-      <c r="F33" t="s">
-        <v>37</v>
-      </c>
       <c r="G33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1339,17 +1379,17 @@
       <c r="C34" t="s">
         <v>8</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>55</v>
       </c>
-      <c r="F34" t="s">
-        <v>37</v>
-      </c>
       <c r="G34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1359,70 +1399,250 @@
       <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>52</v>
       </c>
-      <c r="F35" t="s">
-        <v>37</v>
-      </c>
       <c r="G35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
         <v>93</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
         <v>93</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
         <v>93</v>
       </c>
-      <c r="D38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>92</v>
       </c>
-      <c r="B39" t="s">
-        <v>99</v>
-      </c>
       <c r="C39" t="s">
         <v>93</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" t="s">
+        <v>106</v>
+      </c>
+      <c r="E52" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1435,7 +1655,7 @@
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rerunning DEGs and updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E1C2C-69FA-48EC-B37C-92218463ECAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -362,12 +356,18 @@
   </si>
   <si>
     <t>2022-06-23 16-04-56</t>
+  </si>
+  <si>
+    <t>2022-06-23 16-26-53</t>
+  </si>
+  <si>
+    <t>2022-06-23 16-28-33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -672,18 +672,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,6 +1624,12 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
       <c r="C51" t="s">
         <v>23</v>
       </c>
@@ -1635,6 +1641,12 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
       <c r="C52" t="s">
         <v>23</v>
       </c>
@@ -1651,7 +1663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Running temps and updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29DD471-5CF6-41A6-88F9-D13C01510F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
     <sheet name="SCTv2 pipeline runtime" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -352,22 +368,49 @@
     <t>N</t>
   </si>
   <si>
-    <t>2022-06-23 16-03-44</t>
-  </si>
-  <si>
-    <t>2022-06-23 16-04-56</t>
-  </si>
-  <si>
     <t>2022-06-23 16-26-53</t>
   </si>
   <si>
     <t>2022-06-23 16-28-33</t>
+  </si>
+  <si>
+    <t>old postSelection</t>
+  </si>
+  <si>
+    <t>new postSelection</t>
+  </si>
+  <si>
+    <t>A+C</t>
+  </si>
+  <si>
+    <t>oldPostSelect</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 08-55-17</t>
+  </si>
+  <si>
+    <t>oldSelect</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 08-58-57</t>
+  </si>
+  <si>
+    <t>newPostSelect</t>
+  </si>
+  <si>
+    <t>newSelect</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 09-04-40</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 09-07-27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -672,18 +715,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1637,7 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
@@ -1611,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
         <v>23</v>
@@ -1628,7 +1671,7 @@
         <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
@@ -1645,7 +1688,7 @@
         <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
         <v>23</v>
@@ -1655,6 +1698,118 @@
       </c>
       <c r="E52" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>106</v>
+      </c>
+      <c r="E56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1663,7 +1818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Run temps and updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29DD471-5CF6-41A6-88F9-D13C01510F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
     <sheet name="SCTv2 pipeline runtime" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -405,12 +399,21 @@
   </si>
   <si>
     <t>SingleR_RData_2022-06-24 09-07-27</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>2022-06-24 10-26-27</t>
+  </si>
+  <si>
+    <t>2022-06-24 10-27-42</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -715,18 +718,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1671,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
         <v>110</v>
@@ -1685,7 +1688,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="B52" t="s">
         <v>111</v>
@@ -1701,6 +1704,12 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>124</v>
+      </c>
       <c r="C53" t="s">
         <v>23</v>
       </c>
@@ -1712,6 +1721,12 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
       <c r="C54" t="s">
         <v>23</v>
       </c>
@@ -1818,7 +1833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Runing new temps and updated run log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004270A8-7B05-4503-91CC-C86808A8CD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -15,22 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -362,12 +358,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>2022-06-23 16-26-53</t>
-  </si>
-  <si>
-    <t>2022-06-23 16-28-33</t>
-  </si>
-  <si>
     <t>old postSelection</t>
   </si>
   <si>
@@ -380,40 +370,55 @@
     <t>oldPostSelect</t>
   </si>
   <si>
-    <t>SingleR_RData_2022-06-24 08-55-17</t>
-  </si>
-  <si>
     <t>oldSelect</t>
   </si>
   <si>
-    <t>SingleR_RData_2022-06-24 08-58-57</t>
-  </si>
-  <si>
     <t>newPostSelect</t>
   </si>
   <si>
     <t>newSelect</t>
   </si>
   <si>
-    <t>SingleR_RData_2022-06-24 09-04-40</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-06-24 09-07-27</t>
-  </si>
-  <si>
-    <t>HD</t>
-  </si>
-  <si>
     <t>2022-06-24 10-26-27</t>
   </si>
   <si>
     <t>2022-06-24 10-27-42</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 11-22-36</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 11-24-14</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 11-27-07</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-06-24 11-30-36</t>
+  </si>
+  <si>
+    <t>KS visualization</t>
+  </si>
+  <si>
+    <t>R Kriegstien</t>
+  </si>
+  <si>
+    <t>2022-06-24 12-05-48</t>
+  </si>
+  <si>
+    <t>2022-06-24 12-08-22</t>
+  </si>
+  <si>
+    <t>2022-06-24 12-09-57</t>
+  </si>
+  <si>
+    <t>2022-06-24 12-11-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -718,18 +723,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,10 +1676,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
@@ -1688,10 +1693,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
         <v>23</v>
@@ -1708,7 +1713,7 @@
         <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
@@ -1717,7 +1722,7 @@
         <v>102</v>
       </c>
       <c r="E53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1725,7 +1730,7 @@
         <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -1734,7 +1739,7 @@
         <v>102</v>
       </c>
       <c r="E54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1745,7 +1750,7 @@
         <v>106</v>
       </c>
       <c r="E55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,7 +1761,7 @@
         <v>106</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1764,16 +1769,16 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1781,16 +1786,16 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
       </c>
       <c r="D58" t="s">
+        <v>112</v>
+      </c>
+      <c r="E58" t="s">
         <v>114</v>
-      </c>
-      <c r="E58" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,16 +1803,16 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E59" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1815,16 +1820,208 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="D60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" t="s">
         <v>114</v>
       </c>
-      <c r="E60" t="s">
-        <v>120</v>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" t="s">
+        <v>112</v>
+      </c>
+      <c r="E66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" t="s">
+        <v>123</v>
+      </c>
+      <c r="D68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E68" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" t="s">
+        <v>123</v>
+      </c>
+      <c r="D69" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" t="s">
+        <v>106</v>
+      </c>
+      <c r="E70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+      <c r="D71" t="s">
+        <v>106</v>
+      </c>
+      <c r="E71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" t="s">
+        <v>123</v>
+      </c>
+      <c r="D72" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1833,7 +2030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Run new temps and updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004270A8-7B05-4503-91CC-C86808A8CD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -413,12 +407,21 @@
   </si>
   <si>
     <t>2022-06-24 12-11-01</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>2022-06-24 14-42-15</t>
+  </si>
+  <si>
+    <t>2022-06-24 14-43-31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -723,18 +726,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1713,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
         <v>117</v>
@@ -1727,7 +1730,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="B54" t="s">
         <v>118</v>
@@ -1743,6 +1746,12 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>130</v>
+      </c>
       <c r="C55" t="s">
         <v>23</v>
       </c>
@@ -1754,6 +1763,12 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" t="s">
+        <v>131</v>
+      </c>
       <c r="C56" t="s">
         <v>23</v>
       </c>
@@ -2030,7 +2045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Cleaned up scripts folder, added temps and updated run log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0DEB34-7CF9-4CAF-A659-7B745CDC9ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
-    <sheet name="SCTv2 pipeline runtime" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -214,63 +219,9 @@
     <t>SCTv2 corrected BL_A + BL_C old post selection</t>
   </si>
   <si>
-    <t>script</t>
-  </si>
-  <si>
-    <t>BL_N</t>
-  </si>
-  <si>
-    <t>BL_A</t>
-  </si>
-  <si>
-    <t>BL_C</t>
-  </si>
-  <si>
-    <t>in parallel</t>
-  </si>
-  <si>
-    <t>integration old selection</t>
-  </si>
-  <si>
-    <t>integration new selection</t>
-  </si>
-  <si>
-    <t>BL_N + BL_C</t>
-  </si>
-  <si>
-    <t>BL_A + BL_C</t>
-  </si>
-  <si>
-    <t>time (min)</t>
-  </si>
-  <si>
-    <t>annotation old selection</t>
-  </si>
-  <si>
-    <t>annotation old post selection</t>
-  </si>
-  <si>
-    <t>annotation new post selection</t>
-  </si>
-  <si>
-    <t>annotation new selection</t>
-  </si>
-  <si>
-    <t>individual + integration</t>
-  </si>
-  <si>
     <t>sample(s)</t>
   </si>
   <si>
-    <t>278/515</t>
-  </si>
-  <si>
-    <t>DEGs</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>SCTv2 corrected BL_N + BL_C old post selection</t>
   </si>
   <si>
@@ -328,9 +279,6 @@
     <t>SCTv2 preselection aggrTrue maxLabelScore</t>
   </si>
   <si>
-    <t>A + C</t>
-  </si>
-  <si>
     <t>old selection</t>
   </si>
   <si>
@@ -340,9 +288,6 @@
     <t>Pipe_SCTv2_23-06</t>
   </si>
   <si>
-    <t>N + C</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -373,42 +318,9 @@
     <t>newSelect</t>
   </si>
   <si>
-    <t>2022-06-24 10-26-27</t>
-  </si>
-  <si>
-    <t>2022-06-24 10-27-42</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-06-24 11-22-36</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-06-24 11-24-14</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-06-24 11-27-07</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-06-24 11-30-36</t>
-  </si>
-  <si>
     <t>KS visualization</t>
   </si>
   <si>
-    <t>R Kriegstien</t>
-  </si>
-  <si>
-    <t>2022-06-24 12-05-48</t>
-  </si>
-  <si>
-    <t>2022-06-24 12-08-22</t>
-  </si>
-  <si>
-    <t>2022-06-24 12-09-57</t>
-  </si>
-  <si>
-    <t>2022-06-24 12-11-01</t>
-  </si>
-  <si>
     <t>HD</t>
   </si>
   <si>
@@ -416,12 +328,39 @@
   </si>
   <si>
     <t>2022-06-24 14-43-31</t>
+  </si>
+  <si>
+    <t>N+C</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-35-25</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-48-05</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-48-30</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-49-28</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-50-17</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-50-51</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-51-30</t>
+  </si>
+  <si>
+    <t>2022-06-24 16-52-07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,9 +390,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,18 +664,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1294,7 +1232,7 @@
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
@@ -1334,7 +1272,7 @@
         <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="G29" t="s">
         <v>37</v>
@@ -1368,13 +1306,13 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G31" t="s">
         <v>37</v>
@@ -1388,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -1408,7 +1346,7 @@
         <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
@@ -1428,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1448,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -1465,63 +1403,63 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1529,16 +1467,16 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1546,16 +1484,16 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
         <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1563,16 +1501,16 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
         <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1580,16 +1518,16 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1597,16 +1535,16 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1614,16 +1552,16 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1631,16 +1569,16 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1648,16 +1586,16 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1665,16 +1603,16 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
         <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,16 +1620,16 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1699,50 +1637,50 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C52" t="s">
         <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E53" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E54" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1750,16 +1688,16 @@
         <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
       </c>
       <c r="D55" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1767,16 +1705,16 @@
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
         <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E56" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,16 +1722,16 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E57" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1801,16 +1739,16 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E58" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,16 +1756,16 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1835,16 +1773,16 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1852,16 +1790,16 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E61" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1869,16 +1807,16 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E62" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1886,16 +1824,16 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E63" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1903,316 +1841,288 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E64" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D65" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E65" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D66" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E66" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D67" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E67" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D68" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E68" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>86</v>
       </c>
       <c r="C69" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D69" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E69" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>124</v>
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>86</v>
       </c>
       <c r="C70" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D70" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E70" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>124</v>
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D71" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E71" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>86</v>
       </c>
       <c r="C72" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D72" t="s">
+        <v>101</v>
+      </c>
+      <c r="E72" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>104</v>
+      </c>
+      <c r="C74" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>102</v>
+      </c>
+      <c r="C75" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" t="s">
+        <v>92</v>
+      </c>
+      <c r="E75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" t="s">
+        <v>92</v>
+      </c>
+      <c r="E76" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
         <v>106</v>
       </c>
-      <c r="E72" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="1">
-        <v>37</v>
-      </c>
-      <c r="E8">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="1">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="1">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="1">
-        <v>278</v>
-      </c>
-      <c r="E12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>82</v>
+      <c r="C77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77" t="s">
+        <v>101</v>
+      </c>
+      <c r="E77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>107</v>
+      </c>
+      <c r="C78" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78" t="s">
+        <v>101</v>
+      </c>
+      <c r="E78" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>108</v>
+      </c>
+      <c r="C79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79" t="s">
+        <v>101</v>
+      </c>
+      <c r="E79" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" t="s">
+        <v>101</v>
+      </c>
+      <c r="E80" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished pipe run and moved files to groupfolder, new temps for running pipe with cel level selection
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB60CC7-02A9-4B53-9F23-0E35FF2EE4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26882DA-BE5C-44E0-ABEC-8B0A7CC63CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -349,6 +349,39 @@
   </si>
   <si>
     <t>Pipe_SCTv2_23-14</t>
+  </si>
+  <si>
+    <t>Rerunning with cel level selection for all marker expression</t>
+  </si>
+  <si>
+    <t>oldSelection</t>
+  </si>
+  <si>
+    <t>newSelection</t>
+  </si>
+  <si>
+    <t>Pipe_29-06</t>
+  </si>
+  <si>
+    <t>Pipe_29-07</t>
+  </si>
+  <si>
+    <t>Pipe_29-08</t>
+  </si>
+  <si>
+    <t>Pipe_29-09</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-01 13-24-47</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-01 13-25-24</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-01 13-26-42</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-01 13-27-20</t>
   </si>
 </sst>
 </file>
@@ -672,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,6 +2158,206 @@
         <v>94</v>
       </c>
     </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>78</v>
+      </c>
+      <c r="E82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>111</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" t="s">
+        <v>92</v>
+      </c>
+      <c r="E83" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>92</v>
+      </c>
+      <c r="E84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>99</v>
+      </c>
+      <c r="E85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>99</v>
+      </c>
+      <c r="E86" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>114</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" t="s">
+        <v>92</v>
+      </c>
+      <c r="E87" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>114</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" t="s">
+        <v>92</v>
+      </c>
+      <c r="E88" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" t="s">
+        <v>99</v>
+      </c>
+      <c r="E89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" t="s">
+        <v>99</v>
+      </c>
+      <c r="E90" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>74</v>
+      </c>
+      <c r="B91" t="s">
+        <v>115</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>92</v>
+      </c>
+      <c r="E91" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>74</v>
+      </c>
+      <c r="B92" t="s">
+        <v>116</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>92</v>
+      </c>
+      <c r="E92" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>74</v>
+      </c>
+      <c r="B93" t="s">
+        <v>117</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>99</v>
+      </c>
+      <c r="E93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>99</v>
+      </c>
+      <c r="E94" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Running pipe and updated log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91243F89-E6C8-419C-AFC2-9A3FBB945CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -354,43 +360,22 @@
     <t>newSelection</t>
   </si>
   <si>
-    <t>Pipe_29-06</t>
-  </si>
-  <si>
-    <t>Pipe_29-07</t>
-  </si>
-  <si>
     <t>Pipe_29-08</t>
   </si>
   <si>
     <t>Pipe_29-09</t>
   </si>
   <si>
-    <t>SingleR_RData_2022-07-01 13-24-47</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-07-01 13-25-24</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-07-01 13-26-42</t>
-  </si>
-  <si>
-    <t>SingleR_RData_2022-07-01 13-27-20</t>
-  </si>
-  <si>
-    <t>2022-07-01 13-49-32</t>
-  </si>
-  <si>
     <t>NL results</t>
   </si>
   <si>
-    <t>2022-07-01 13-51-40</t>
+    <t>results/Kriegstein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,18 +685,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C84" t="s">
         <v>3</v>
@@ -2208,7 +2193,7 @@
         <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
@@ -2225,7 +2210,7 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C86" t="s">
         <v>3</v>
@@ -2242,7 +2227,7 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C87" t="s">
         <v>23</v>
@@ -2259,7 +2244,7 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C88" t="s">
         <v>23</v>
@@ -2273,10 +2258,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B89" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C89" t="s">
         <v>23</v>
@@ -2290,10 +2275,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B90" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C90" t="s">
         <v>23</v>
@@ -2310,7 +2295,7 @@
         <v>74</v>
       </c>
       <c r="B91" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -2327,7 +2312,7 @@
         <v>74</v>
       </c>
       <c r="B92" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -2344,7 +2329,7 @@
         <v>74</v>
       </c>
       <c r="B93" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C93" t="s">
         <v>8</v>
@@ -2361,7 +2346,7 @@
         <v>74</v>
       </c>
       <c r="B94" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -2370,6 +2355,142 @@
         <v>99</v>
       </c>
       <c r="E94" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" t="s">
+        <v>97</v>
+      </c>
+      <c r="D95" t="s">
+        <v>92</v>
+      </c>
+      <c r="E95" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" t="s">
+        <v>112</v>
+      </c>
+      <c r="C96" t="s">
+        <v>97</v>
+      </c>
+      <c r="D96" t="s">
+        <v>92</v>
+      </c>
+      <c r="E96" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" t="s">
+        <v>112</v>
+      </c>
+      <c r="C97" t="s">
+        <v>97</v>
+      </c>
+      <c r="D97" t="s">
+        <v>99</v>
+      </c>
+      <c r="E97" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" t="s">
+        <v>97</v>
+      </c>
+      <c r="D98" t="s">
+        <v>99</v>
+      </c>
+      <c r="E98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" t="s">
+        <v>112</v>
+      </c>
+      <c r="C99" t="s">
+        <v>62</v>
+      </c>
+      <c r="D99" t="s">
+        <v>92</v>
+      </c>
+      <c r="E99" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" t="s">
+        <v>62</v>
+      </c>
+      <c r="D100" t="s">
+        <v>92</v>
+      </c>
+      <c r="E100" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" t="s">
+        <v>112</v>
+      </c>
+      <c r="C101" t="s">
+        <v>62</v>
+      </c>
+      <c r="D101" t="s">
+        <v>99</v>
+      </c>
+      <c r="E101" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" t="s">
+        <v>112</v>
+      </c>
+      <c r="C102" t="s">
+        <v>62</v>
+      </c>
+      <c r="D102" t="s">
+        <v>99</v>
+      </c>
+      <c r="E102" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
temps for pipe_29-06 into own folder, new temps for finishing A C N pipe_23-06, updated run log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91243F89-E6C8-419C-AFC2-9A3FBB945CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF0F165-748A-4BA1-802C-3886BC097DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -370,6 +370,15 @@
   </si>
   <si>
     <t>results/Kriegstein</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-04 11-47-53</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-04 11-49-06</t>
+  </si>
+  <si>
+    <t>SingleR_RData_2022-07-04 11-49-39</t>
   </si>
 </sst>
 </file>
@@ -693,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,6 +2503,48 @@
         <v>110</v>
       </c>
     </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>74</v>
+      </c>
+      <c r="B104" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>74</v>
+      </c>
+      <c r="B105" t="s">
+        <v>116</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>74</v>
+      </c>
+      <c r="B106" t="s">
+        <v>117</v>
+      </c>
+      <c r="C106" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New temps and updated run log
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\Single Cell RNA Sequencing\Seurat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF0F165-748A-4BA1-802C-3886BC097DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="logs" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -379,12 +373,21 @@
   </si>
   <si>
     <t>SingleR_RData_2022-07-04 11-49-39</t>
+  </si>
+  <si>
+    <t>2022-07-04 11-56-43</t>
+  </si>
+  <si>
+    <t>2022-07-04 11-58-43</t>
+  </si>
+  <si>
+    <t>2022-07-04 11-59-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -694,18 +697,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,6 +2548,48 @@
         <v>89</v>
       </c>
     </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107" t="s">
+        <v>118</v>
+      </c>
+      <c r="C107" t="s">
+        <v>23</v>
+      </c>
+      <c r="D107" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108" t="s">
+        <v>23</v>
+      </c>
+      <c r="D108" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>44</v>
+      </c>
+      <c r="B109" t="s">
+        <v>120</v>
+      </c>
+      <c r="C109" t="s">
+        <v>23</v>
+      </c>
+      <c r="D109" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New temps and updated runlog
</commit_message>
<xml_diff>
--- a/Seurat/results log.xlsx
+++ b/Seurat/results log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -373,15 +373,6 @@
   </si>
   <si>
     <t>SingleR_RData_2022-07-04 11-49-39</t>
-  </si>
-  <si>
-    <t>2022-07-04 11-56-43</t>
-  </si>
-  <si>
-    <t>2022-07-04 11-58-43</t>
-  </si>
-  <si>
-    <t>2022-07-04 11-59-22</t>
   </si>
 </sst>
 </file>
@@ -697,7 +688,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -707,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,10 +2541,10 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="C107" t="s">
         <v>23</v>
@@ -2564,10 +2555,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="C108" t="s">
         <v>23</v>
@@ -2578,10 +2569,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="C109" t="s">
         <v>23</v>

</xml_diff>